<commit_message>
Added EDA for loan vol, grade, FICO, etc
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmtrinh/Desktop/Berkeley-PC-ML-AI/Capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FDE0BD-A399-7244-91FE-D0157CD5D5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C82481-ECBC-7A4F-9BA9-42947EB2CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16040" yWindow="1740" windowWidth="38820" windowHeight="22100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41120" yWindow="2760" windowWidth="30880" windowHeight="22100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1133,7 +1133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1328,6 +1328,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1566,7 +1572,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1583,8 +1589,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1986,8 +1993,8 @@
   <dimension ref="A1:C154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25:A26"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" activeCellId="3" sqref="A61 A62 A63 A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2015,7 +2022,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="9" t="s">
         <v>217</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2023,7 +2030,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2039,7 +2046,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2047,7 +2054,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2055,7 +2062,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2063,7 +2070,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2071,7 +2078,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="9" t="s">
         <v>218</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2079,7 +2086,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>219</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2087,7 +2094,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2103,7 +2110,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2111,7 +2118,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2120,7 +2127,7 @@
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="9" t="s">
         <v>220</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2129,7 +2136,7 @@
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2137,7 +2144,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2145,7 +2152,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>177</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2153,7 +2160,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2161,7 +2168,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2169,7 +2176,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>153</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2177,7 +2184,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2185,7 +2192,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2209,7 +2216,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2217,7 +2224,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2234,7 +2241,7 @@
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>199</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2251,7 +2258,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>209</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2259,7 +2266,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2267,7 +2274,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2275,7 +2282,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2283,7 +2290,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2291,7 +2298,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2299,7 +2306,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2307,7 +2314,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2315,7 +2322,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2339,7 +2346,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2347,7 +2354,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2355,7 +2362,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="7" t="s">
         <v>205</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2363,7 +2370,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2371,7 +2378,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="9" t="s">
         <v>221</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2379,7 +2386,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2387,7 +2394,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2395,7 +2402,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2411,7 +2418,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2419,7 +2426,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2427,7 +2434,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2435,7 +2442,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="9" t="s">
         <v>195</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2443,7 +2450,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="9" t="s">
         <v>223</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2451,7 +2458,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="9" t="s">
         <v>224</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2459,7 +2466,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="9" t="s">
         <v>226</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2467,7 +2474,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="9" t="s">
         <v>227</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2483,7 +2490,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="9" t="s">
         <v>97</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2491,7 +2498,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2499,7 +2506,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2507,7 +2514,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2515,7 +2522,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2523,7 +2530,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2531,7 +2538,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2539,7 +2546,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2547,7 +2554,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2555,7 +2562,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2579,7 +2586,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2587,7 +2594,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2595,7 +2602,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2667,7 +2674,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2675,7 +2682,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="9" t="s">
         <v>228</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -2691,7 +2698,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -2699,7 +2706,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2707,7 +2714,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -2731,7 +2738,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -2739,7 +2746,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -2747,7 +2754,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2755,7 +2762,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -2763,7 +2770,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="s">
+      <c r="A96" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2779,7 +2786,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="9" t="s">
         <v>121</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -2787,7 +2794,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -2795,7 +2802,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -2803,7 +2810,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -2811,7 +2818,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="9" t="s">
         <v>229</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -2827,7 +2834,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="9" t="s">
         <v>230</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -2843,7 +2850,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -2891,7 +2898,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="9" t="s">
         <v>156</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -2907,7 +2914,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="9" t="s">
+      <c r="A114" s="8" t="s">
         <v>216</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -2915,7 +2922,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="9" t="s">
+      <c r="A115" s="7" t="s">
         <v>179</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -2923,7 +2930,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="9" t="s">
         <v>169</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -2931,7 +2938,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="9" t="s">
+      <c r="A117" s="8" t="s">
         <v>232</v>
       </c>
       <c r="B117" s="1" t="s">

</xml_diff>

<commit_message>
Added notebook for ML classification models
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmtrinh/Desktop/Berkeley-PC-ML-AI/Capstone/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmtrinh/Desktop/Berkeley-PC-ML-AI/Capstone/loan-default-prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C82481-ECBC-7A4F-9BA9-42947EB2CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF38F4D-62D1-C048-A2A8-814F72BB08CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41120" yWindow="2760" windowWidth="30880" windowHeight="22100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18560" yWindow="900" windowWidth="41120" windowHeight="24280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1993,8 +1993,8 @@
   <dimension ref="A1:C154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" activeCellId="3" sqref="A61 A62 A63 A64"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2014,7 +2014,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>213</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2094,7 +2094,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2136,7 +2136,7 @@
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2370,7 +2370,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">

</xml_diff>